<commit_message>
update packages w/ fixed metadata hash
</commit_message>
<xml_diff>
--- a/mappings/package_eforms_sdk1.11_epo4.0/transformation/conceptual_mappings.xlsx
+++ b/mappings/package_eforms_sdk1.11_epo4.0/transformation/conceptual_mappings.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1714" uniqueCount="1055">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1715" uniqueCount="1055">
   <si>
     <t>Field</t>
   </si>
@@ -364,6 +364,9 @@
     <t>OPT-301-Part-FiscalLegis</t>
   </si>
   <si>
+    <t>BT-1501(p)-Contract</t>
+  </si>
+  <si>
     <t>OPT-110-Part-FiscalLegis</t>
   </si>
   <si>
@@ -538,9 +541,6 @@
     <t>ND-ModifiedSection</t>
   </si>
   <si>
-    <t>BT-1501(p)-Contract</t>
-  </si>
-  <si>
     <t>BT-202-Contract</t>
   </si>
   <si>
@@ -871,6 +871,9 @@
     <t>Fiscal Legislation Organization Technical Identifier Reference</t>
   </si>
   <si>
+    <t>Modified Notice Part Reference</t>
+  </si>
+  <si>
     <t>URL to Fiscal Legislation</t>
   </si>
   <si>
@@ -997,9 +1000,6 @@
     <t>Modification Reason Description</t>
   </si>
   <si>
-    <t>Modified Notice Part Reference</t>
-  </si>
-  <si>
     <t>Modification Description</t>
   </si>
   <si>
@@ -1303,6 +1303,9 @@
     <t>OPT-301</t>
   </si>
   <si>
+    <t>BT-1501</t>
+  </si>
+  <si>
     <t>OPT-110</t>
   </si>
   <si>
@@ -1384,9 +1387,6 @@
     <t>BT-798</t>
   </si>
   <si>
-    <t>BT-1501</t>
-  </si>
-  <si>
     <t>BT-799</t>
   </si>
   <si>
@@ -1702,6 +1702,9 @@
     <t>/*/cac:ProcurementProjectLot[cbc:ID/@schemeName='Part']/cac:TenderingTerms/cac:FiscalLegislationDocumentReference/cac:IssuerParty/cac:PartyIdentification/cbc:ID</t>
   </si>
   <si>
+    <t>/*/ext:UBLExtensions/ext:UBLExtension/ext:ExtensionContent/efext:EformsExtension/efac:ContractModification/efac:Change/efac:ChangedSection/efbc:ChangedSectionIdentifier</t>
+  </si>
+  <si>
     <t>/*/cac:ProcurementProjectLot[cbc:ID/@schemeName='Part']/cac:TenderingTerms/cac:FiscalLegislationDocumentReference/cac:Attachment/cac:ExternalReference/cbc:URI</t>
   </si>
   <si>
@@ -1874,9 +1877,6 @@
   </si>
   <si>
     <t>/*/ext:UBLExtensions/ext:UBLExtension/ext:ExtensionContent/efext:EformsExtension/efac:ContractModification/efac:Change/efac:ChangedSection</t>
-  </si>
-  <si>
-    <t>/*/ext:UBLExtensions/ext:UBLExtension/ext:ExtensionContent/efext:EformsExtension/efac:ContractModification/efac:Change/efac:ChangedSection/efbc:ChangedSectionIdentifier</t>
   </si>
   <si>
     <t>/*/ext:UBLExtensions/ext:UBLExtension/ext:ExtensionContent/efext:EformsExtension/efac:ContractModification/efac:Change/efbc:ChangeDescription</t>
@@ -2301,6 +2301,9 @@
     <t>epo-not:PlanningNotice / epo:TaxInformationProvider / org:Organization</t>
   </si>
   <si>
+    <t>epo-con:ContractModificationInformation / adms:Identifier / rdf:langString</t>
+  </si>
+  <si>
     <t>epo-not:PlanningNotice / epo:EnvironmentalProtectionInformationProvider / epo:ProcurementObject</t>
   </si>
   <si>
@@ -2464,9 +2467,6 @@
   </si>
   <si>
     <t>epo-con:ContractModificationInformation / rdf:langString</t>
-  </si>
-  <si>
-    <t>epo-con:ContractModificationInformation / adms:Identifier / rdf:langString</t>
   </si>
   <si>
     <t>epo:Tender / epo:ConcessionEstimate / epo:MonetaryValue / at-voc:currency</t>
@@ -2628,6 +2628,9 @@
     <t>?this epo:announcesRole / epo:playedBy ?value .</t>
   </si>
   <si>
+    <t>?this epo:relatesToEFormSectionIdentifier / skos:notation ?value .</t>
+  </si>
+  <si>
     <t>?this epo:foreseesProcurementObject / epo:hasAdditionalInformation ?value .</t>
   </si>
   <si>
@@ -2719,9 +2722,6 @@
   </si>
   <si>
     <t>?this epo:hasModificationReasonDescription ?value</t>
-  </si>
-  <si>
-    <t>?this epo:relatesToEFormSectionIdentifier / skos:notation ?value .</t>
   </si>
   <si>
     <t>?this epo:hasModificationDescription ?value</t>
@@ -2825,13 +2825,13 @@
     <t>Sent to EPO WG</t>
   </si>
   <si>
+    <t>For OP consultation</t>
+  </si>
+  <si>
     <t>Approved by first OP reviewer</t>
   </si>
   <si>
     <t>For internal review</t>
-  </si>
-  <si>
-    <t>For OP consultation</t>
   </si>
   <si>
     <t>This mapping applies only for Planning Notices (eForm subtypes 1-9, E2 and T01).
@@ -5414,6 +5414,12 @@
       </c>
     </row>
     <row r="74" spans="1:12">
+      <c r="A74" t="s">
+        <v>20</v>
+      </c>
+      <c r="B74" t="s">
+        <v>20</v>
+      </c>
       <c r="C74" t="s">
         <v>115</v>
       </c>
@@ -5426,11 +5432,14 @@
       <c r="G74" t="s">
         <v>561</v>
       </c>
+      <c r="I74" t="s">
+        <v>760</v>
+      </c>
+      <c r="J74" t="s">
+        <v>868</v>
+      </c>
       <c r="K74" t="s">
-        <v>932</v>
-      </c>
-      <c r="L74" t="s">
-        <v>950</v>
+        <v>933</v>
       </c>
     </row>
     <row r="75" spans="1:12">
@@ -5454,66 +5463,57 @@
       </c>
     </row>
     <row r="76" spans="1:12">
-      <c r="A76" t="s">
-        <v>47</v>
-      </c>
       <c r="C76" t="s">
         <v>117</v>
       </c>
+      <c r="D76" t="s">
+        <v>286</v>
+      </c>
+      <c r="E76" t="s">
+        <v>430</v>
+      </c>
       <c r="G76" t="s">
         <v>563</v>
       </c>
-      <c r="I76" t="s">
-        <v>760</v>
-      </c>
-      <c r="J76" t="s">
-        <v>865</v>
-      </c>
       <c r="K76" t="s">
-        <v>929</v>
+        <v>932</v>
+      </c>
+      <c r="L76" t="s">
+        <v>950</v>
       </c>
     </row>
     <row r="77" spans="1:12">
+      <c r="A77" t="s">
+        <v>47</v>
+      </c>
       <c r="C77" t="s">
         <v>118</v>
       </c>
-      <c r="D77" t="s">
-        <v>286</v>
-      </c>
-      <c r="E77" t="s">
-        <v>427</v>
-      </c>
       <c r="G77" t="s">
         <v>564</v>
       </c>
-      <c r="H77" t="s">
-        <v>706</v>
-      </c>
       <c r="I77" t="s">
         <v>761</v>
       </c>
       <c r="J77" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="K77" t="s">
-        <v>931</v>
-      </c>
-      <c r="L77" t="s">
-        <v>951</v>
+        <v>929</v>
       </c>
     </row>
     <row r="78" spans="1:12">
       <c r="C78" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D78" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="E78" t="s">
         <v>427</v>
       </c>
       <c r="G78" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="H78" t="s">
         <v>706</v>
@@ -5522,13 +5522,13 @@
         <v>762</v>
       </c>
       <c r="J78" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="K78" t="s">
         <v>931</v>
       </c>
       <c r="L78" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="79" spans="1:12">
@@ -5539,16 +5539,25 @@
         <v>287</v>
       </c>
       <c r="E79" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="G79" t="s">
         <v>565</v>
       </c>
+      <c r="H79" t="s">
+        <v>706</v>
+      </c>
+      <c r="I79" t="s">
+        <v>763</v>
+      </c>
+      <c r="J79" t="s">
+        <v>867</v>
+      </c>
       <c r="K79" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="L79" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
     </row>
     <row r="80" spans="1:12">
@@ -5572,66 +5581,57 @@
       </c>
     </row>
     <row r="81" spans="1:12">
-      <c r="A81" t="s">
-        <v>47</v>
-      </c>
       <c r="C81" t="s">
         <v>121</v>
       </c>
+      <c r="D81" t="s">
+        <v>289</v>
+      </c>
+      <c r="E81" t="s">
+        <v>432</v>
+      </c>
       <c r="G81" t="s">
         <v>567</v>
       </c>
-      <c r="I81" t="s">
-        <v>763</v>
-      </c>
-      <c r="J81" t="s">
-        <v>865</v>
-      </c>
       <c r="K81" t="s">
-        <v>929</v>
+        <v>932</v>
+      </c>
+      <c r="L81" t="s">
+        <v>950</v>
       </c>
     </row>
     <row r="82" spans="1:12">
+      <c r="A82" t="s">
+        <v>47</v>
+      </c>
       <c r="C82" t="s">
         <v>122</v>
       </c>
-      <c r="D82" t="s">
-        <v>289</v>
-      </c>
-      <c r="E82" t="s">
-        <v>427</v>
-      </c>
       <c r="G82" t="s">
         <v>568</v>
       </c>
-      <c r="H82" t="s">
-        <v>706</v>
-      </c>
       <c r="I82" t="s">
         <v>764</v>
       </c>
       <c r="J82" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="K82" t="s">
-        <v>931</v>
-      </c>
-      <c r="L82" t="s">
-        <v>953</v>
+        <v>929</v>
       </c>
     </row>
     <row r="83" spans="1:12">
       <c r="C83" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D83" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="E83" t="s">
         <v>427</v>
       </c>
       <c r="G83" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="H83" t="s">
         <v>706</v>
@@ -5640,13 +5640,13 @@
         <v>765</v>
       </c>
       <c r="J83" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="K83" t="s">
         <v>931</v>
       </c>
       <c r="L83" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="84" spans="1:12">
@@ -5657,16 +5657,25 @@
         <v>290</v>
       </c>
       <c r="E84" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="G84" t="s">
         <v>569</v>
       </c>
+      <c r="H84" t="s">
+        <v>706</v>
+      </c>
+      <c r="I84" t="s">
+        <v>766</v>
+      </c>
+      <c r="J84" t="s">
+        <v>867</v>
+      </c>
       <c r="K84" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="L84" t="s">
-        <v>950</v>
+        <v>954</v>
       </c>
     </row>
     <row r="85" spans="1:12">
@@ -5697,68 +5706,59 @@
         <v>292</v>
       </c>
       <c r="E86" t="s">
-        <v>427</v>
+        <v>434</v>
       </c>
       <c r="G86" t="s">
         <v>571</v>
       </c>
-      <c r="H86" t="s">
-        <v>707</v>
-      </c>
-      <c r="I86" t="s">
-        <v>766</v>
-      </c>
-      <c r="J86" t="s">
-        <v>865</v>
-      </c>
       <c r="K86" t="s">
-        <v>929</v>
+        <v>932</v>
       </c>
       <c r="L86" t="s">
-        <v>955</v>
+        <v>950</v>
       </c>
     </row>
     <row r="87" spans="1:12">
       <c r="C87" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D87" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="E87" t="s">
         <v>427</v>
       </c>
       <c r="G87" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="H87" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="I87" t="s">
         <v>767</v>
       </c>
       <c r="J87" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="K87" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="L87" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="88" spans="1:12">
       <c r="C88" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D88" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="E88" t="s">
         <v>427</v>
       </c>
       <c r="G88" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="H88" t="s">
         <v>708</v>
@@ -5767,13 +5767,13 @@
         <v>768</v>
       </c>
       <c r="J88" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="K88" t="s">
         <v>931</v>
       </c>
       <c r="L88" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="89" spans="1:12">
@@ -5789,57 +5789,57 @@
       <c r="G89" t="s">
         <v>572</v>
       </c>
+      <c r="H89" t="s">
+        <v>708</v>
+      </c>
       <c r="I89" t="s">
         <v>769</v>
       </c>
       <c r="J89" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="K89" t="s">
-        <v>929</v>
+        <v>931</v>
+      </c>
+      <c r="L89" t="s">
+        <v>957</v>
       </c>
     </row>
     <row r="90" spans="1:12">
       <c r="C90" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D90" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E90" t="s">
         <v>427</v>
       </c>
       <c r="G90" t="s">
-        <v>572</v>
-      </c>
-      <c r="H90" t="s">
-        <v>709</v>
+        <v>573</v>
       </c>
       <c r="I90" t="s">
         <v>770</v>
       </c>
       <c r="J90" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="K90" t="s">
-        <v>931</v>
-      </c>
-      <c r="L90" t="s">
-        <v>958</v>
+        <v>929</v>
       </c>
     </row>
     <row r="91" spans="1:12">
       <c r="C91" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D91" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E91" t="s">
         <v>427</v>
       </c>
       <c r="G91" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="H91" t="s">
         <v>709</v>
@@ -5848,13 +5848,13 @@
         <v>771</v>
       </c>
       <c r="J91" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="K91" t="s">
         <v>931</v>
       </c>
       <c r="L91" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="92" spans="1:12">
@@ -5865,68 +5865,80 @@
         <v>294</v>
       </c>
       <c r="E92" t="s">
-        <v>434</v>
-      </c>
-      <c r="F92" t="s">
-        <v>489</v>
+        <v>427</v>
       </c>
       <c r="G92" t="s">
         <v>573</v>
       </c>
+      <c r="H92" t="s">
+        <v>709</v>
+      </c>
       <c r="I92" t="s">
         <v>772</v>
       </c>
       <c r="J92" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="K92" t="s">
-        <v>933</v>
+        <v>931</v>
+      </c>
+      <c r="L92" t="s">
+        <v>959</v>
       </c>
     </row>
     <row r="93" spans="1:12">
       <c r="C93" t="s">
         <v>128</v>
       </c>
+      <c r="D93" t="s">
+        <v>295</v>
+      </c>
+      <c r="E93" t="s">
+        <v>435</v>
+      </c>
+      <c r="F93" t="s">
+        <v>489</v>
+      </c>
       <c r="G93" t="s">
         <v>574</v>
       </c>
+      <c r="I93" t="s">
+        <v>773</v>
+      </c>
+      <c r="J93" t="s">
+        <v>869</v>
+      </c>
       <c r="K93" t="s">
-        <v>930</v>
+        <v>934</v>
       </c>
     </row>
     <row r="94" spans="1:12">
-      <c r="A94" t="s">
-        <v>46</v>
-      </c>
       <c r="C94" t="s">
         <v>129</v>
       </c>
-      <c r="D94" t="s">
-        <v>295</v>
-      </c>
-      <c r="E94" t="s">
-        <v>435</v>
-      </c>
-      <c r="F94" t="s">
-        <v>488</v>
-      </c>
       <c r="G94" t="s">
         <v>575</v>
       </c>
-      <c r="I94" t="s">
-        <v>773</v>
-      </c>
-      <c r="J94" t="s">
-        <v>869</v>
-      </c>
       <c r="K94" t="s">
-        <v>933</v>
+        <v>930</v>
       </c>
     </row>
     <row r="95" spans="1:12">
+      <c r="A95" t="s">
+        <v>46</v>
+      </c>
       <c r="C95" t="s">
         <v>130</v>
       </c>
+      <c r="D95" t="s">
+        <v>296</v>
+      </c>
+      <c r="E95" t="s">
+        <v>436</v>
+      </c>
+      <c r="F95" t="s">
+        <v>488</v>
+      </c>
       <c r="G95" t="s">
         <v>576</v>
       </c>
@@ -5937,19 +5949,13 @@
         <v>870</v>
       </c>
       <c r="K95" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
     </row>
     <row r="96" spans="1:12">
       <c r="C96" t="s">
         <v>131</v>
       </c>
-      <c r="D96" t="s">
-        <v>296</v>
-      </c>
-      <c r="E96" t="s">
-        <v>436</v>
-      </c>
       <c r="G96" t="s">
         <v>577</v>
       </c>
@@ -5960,10 +5966,7 @@
         <v>871</v>
       </c>
       <c r="K96" t="s">
-        <v>933</v>
-      </c>
-      <c r="L96" t="s">
-        <v>960</v>
+        <v>934</v>
       </c>
     </row>
     <row r="97" spans="1:12">
@@ -5971,22 +5974,22 @@
         <v>132</v>
       </c>
       <c r="D97" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="E97" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="G97" t="s">
         <v>578</v>
       </c>
       <c r="I97" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="J97" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="K97" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="L97" t="s">
         <v>960</v>
@@ -5996,17 +5999,26 @@
       <c r="C98" t="s">
         <v>133</v>
       </c>
+      <c r="D98" t="s">
+        <v>297</v>
+      </c>
+      <c r="E98" t="s">
+        <v>437</v>
+      </c>
       <c r="G98" t="s">
         <v>579</v>
       </c>
       <c r="I98" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="J98" t="s">
-        <v>870</v>
+        <v>872</v>
       </c>
       <c r="K98" t="s">
-        <v>933</v>
+        <v>934</v>
+      </c>
+      <c r="L98" t="s">
+        <v>960</v>
       </c>
     </row>
     <row r="99" spans="1:12">
@@ -6016,8 +6028,14 @@
       <c r="G99" t="s">
         <v>580</v>
       </c>
+      <c r="I99" t="s">
+        <v>775</v>
+      </c>
+      <c r="J99" t="s">
+        <v>871</v>
+      </c>
       <c r="K99" t="s">
-        <v>930</v>
+        <v>934</v>
       </c>
     </row>
     <row r="100" spans="1:12">
@@ -6032,37 +6050,37 @@
       </c>
     </row>
     <row r="101" spans="1:12">
-      <c r="A101" t="s">
-        <v>46</v>
-      </c>
       <c r="C101" t="s">
         <v>136</v>
       </c>
-      <c r="D101" t="s">
-        <v>297</v>
-      </c>
-      <c r="E101" t="s">
-        <v>437</v>
-      </c>
       <c r="G101" t="s">
         <v>582</v>
       </c>
       <c r="K101" t="s">
-        <v>932</v>
-      </c>
-      <c r="L101" t="s">
-        <v>961</v>
+        <v>930</v>
       </c>
     </row>
     <row r="102" spans="1:12">
+      <c r="A102" t="s">
+        <v>46</v>
+      </c>
       <c r="C102" t="s">
         <v>137</v>
       </c>
+      <c r="D102" t="s">
+        <v>298</v>
+      </c>
+      <c r="E102" t="s">
+        <v>438</v>
+      </c>
       <c r="G102" t="s">
         <v>583</v>
       </c>
       <c r="K102" t="s">
-        <v>930</v>
+        <v>932</v>
+      </c>
+      <c r="L102" t="s">
+        <v>961</v>
       </c>
     </row>
     <row r="103" spans="1:12">
@@ -6077,29 +6095,20 @@
       </c>
     </row>
     <row r="104" spans="1:12">
-      <c r="A104" t="s">
-        <v>46</v>
-      </c>
       <c r="C104" t="s">
         <v>139</v>
       </c>
-      <c r="D104" t="s">
-        <v>298</v>
-      </c>
-      <c r="E104" t="s">
-        <v>438</v>
-      </c>
       <c r="G104" t="s">
         <v>585</v>
       </c>
       <c r="K104" t="s">
-        <v>932</v>
-      </c>
-      <c r="L104" t="s">
-        <v>962</v>
+        <v>930</v>
       </c>
     </row>
     <row r="105" spans="1:12">
+      <c r="A105" t="s">
+        <v>46</v>
+      </c>
       <c r="C105" t="s">
         <v>140</v>
       </c>
@@ -6112,55 +6121,43 @@
       <c r="G105" t="s">
         <v>586</v>
       </c>
-      <c r="H105" t="s">
-        <v>710</v>
-      </c>
-      <c r="I105" t="s">
-        <v>776</v>
-      </c>
-      <c r="J105" t="s">
-        <v>872</v>
-      </c>
       <c r="K105" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="L105" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="106" spans="1:12">
       <c r="C106" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D106" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E106" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="G106" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="H106" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="I106" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="J106" t="s">
         <v>873</v>
       </c>
       <c r="K106" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="L106" t="s">
         <v>963</v>
       </c>
     </row>
     <row r="107" spans="1:12">
-      <c r="A107" t="s">
-        <v>48</v>
-      </c>
       <c r="C107" t="s">
         <v>141</v>
       </c>
@@ -6173,6 +6170,9 @@
       <c r="G107" t="s">
         <v>587</v>
       </c>
+      <c r="H107" t="s">
+        <v>711</v>
+      </c>
       <c r="I107" t="s">
         <v>777</v>
       </c>
@@ -6180,7 +6180,7 @@
         <v>874</v>
       </c>
       <c r="K107" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="L107" t="s">
         <v>963</v>
@@ -6188,7 +6188,7 @@
     </row>
     <row r="108" spans="1:12">
       <c r="A108" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C108" t="s">
         <v>142</v>
@@ -6209,7 +6209,7 @@
         <v>875</v>
       </c>
       <c r="K108" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="L108" t="s">
         <v>963</v>
@@ -6217,7 +6217,7 @@
     </row>
     <row r="109" spans="1:12">
       <c r="A109" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C109" t="s">
         <v>143</v>
@@ -6232,19 +6232,22 @@
         <v>589</v>
       </c>
       <c r="I109" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="J109" t="s">
         <v>876</v>
       </c>
       <c r="K109" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="L109" t="s">
         <v>963</v>
       </c>
     </row>
     <row r="110" spans="1:12">
+      <c r="A110" t="s">
+        <v>48</v>
+      </c>
       <c r="C110" t="s">
         <v>144</v>
       </c>
@@ -6257,45 +6260,48 @@
       <c r="G110" t="s">
         <v>590</v>
       </c>
+      <c r="I110" t="s">
+        <v>779</v>
+      </c>
+      <c r="J110" t="s">
+        <v>877</v>
+      </c>
       <c r="K110" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="L110" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="111" spans="1:12">
       <c r="C111" t="s">
         <v>145</v>
       </c>
+      <c r="D111" t="s">
+        <v>304</v>
+      </c>
+      <c r="E111" t="s">
+        <v>444</v>
+      </c>
       <c r="G111" t="s">
         <v>591</v>
       </c>
       <c r="K111" t="s">
-        <v>933</v>
+        <v>934</v>
+      </c>
+      <c r="L111" t="s">
+        <v>964</v>
       </c>
     </row>
     <row r="112" spans="1:12">
       <c r="C112" t="s">
         <v>146</v>
       </c>
-      <c r="D112" t="s">
-        <v>304</v>
-      </c>
-      <c r="E112" t="s">
-        <v>444</v>
-      </c>
       <c r="G112" t="s">
         <v>592</v>
       </c>
-      <c r="I112" t="s">
-        <v>779</v>
-      </c>
-      <c r="J112" t="s">
-        <v>877</v>
-      </c>
       <c r="K112" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
     </row>
     <row r="113" spans="2:12">
@@ -6312,13 +6318,13 @@
         <v>593</v>
       </c>
       <c r="I113" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="J113" t="s">
         <v>878</v>
       </c>
       <c r="K113" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
     </row>
     <row r="114" spans="2:12">
@@ -6329,7 +6335,7 @@
         <v>306</v>
       </c>
       <c r="E114" t="s">
-        <v>427</v>
+        <v>446</v>
       </c>
       <c r="G114" t="s">
         <v>594</v>
@@ -6338,39 +6344,36 @@
         <v>780</v>
       </c>
       <c r="J114" t="s">
-        <v>865</v>
+        <v>879</v>
       </c>
       <c r="K114" t="s">
-        <v>929</v>
+        <v>934</v>
       </c>
     </row>
     <row r="115" spans="2:12">
       <c r="C115" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D115" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="E115" t="s">
         <v>427</v>
       </c>
       <c r="G115" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="I115" t="s">
         <v>781</v>
       </c>
       <c r="J115" t="s">
-        <v>870</v>
+        <v>865</v>
       </c>
       <c r="K115" t="s">
-        <v>934</v>
+        <v>929</v>
       </c>
     </row>
     <row r="116" spans="2:12">
-      <c r="B116" t="s">
-        <v>20</v>
-      </c>
       <c r="C116" t="s">
         <v>149</v>
       </c>
@@ -6378,76 +6381,73 @@
         <v>307</v>
       </c>
       <c r="E116" t="s">
-        <v>395</v>
+        <v>427</v>
       </c>
       <c r="G116" t="s">
         <v>595</v>
       </c>
+      <c r="I116" t="s">
+        <v>782</v>
+      </c>
+      <c r="J116" t="s">
+        <v>871</v>
+      </c>
+      <c r="K116" t="s">
+        <v>935</v>
+      </c>
     </row>
     <row r="117" spans="2:12">
+      <c r="B117" t="s">
+        <v>20</v>
+      </c>
       <c r="C117" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D117" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="E117" t="s">
-        <v>427</v>
+        <v>395</v>
       </c>
       <c r="G117" t="s">
-        <v>594</v>
-      </c>
-      <c r="I117" t="s">
-        <v>782</v>
-      </c>
-      <c r="J117" t="s">
-        <v>879</v>
-      </c>
-      <c r="K117" t="s">
-        <v>934</v>
+        <v>596</v>
       </c>
     </row>
     <row r="118" spans="2:12">
       <c r="C118" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D118" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="E118" t="s">
         <v>427</v>
       </c>
       <c r="G118" t="s">
-        <v>594</v>
-      </c>
-      <c r="H118" t="s">
-        <v>712</v>
+        <v>595</v>
       </c>
       <c r="I118" t="s">
         <v>783</v>
       </c>
       <c r="J118" t="s">
-        <v>866</v>
+        <v>880</v>
       </c>
       <c r="K118" t="s">
-        <v>931</v>
-      </c>
-      <c r="L118" t="s">
-        <v>965</v>
+        <v>935</v>
       </c>
     </row>
     <row r="119" spans="2:12">
       <c r="C119" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D119" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="E119" t="s">
         <v>427</v>
       </c>
       <c r="G119" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="H119" t="s">
         <v>712</v>
@@ -6456,125 +6456,125 @@
         <v>784</v>
       </c>
       <c r="J119" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="K119" t="s">
         <v>931</v>
       </c>
       <c r="L119" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="120" spans="2:12">
       <c r="C120" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D120" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E120" t="s">
         <v>427</v>
       </c>
       <c r="G120" t="s">
-        <v>596</v>
+        <v>595</v>
+      </c>
+      <c r="H120" t="s">
+        <v>712</v>
       </c>
       <c r="I120" t="s">
         <v>785</v>
       </c>
       <c r="J120" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="K120" t="s">
-        <v>929</v>
+        <v>931</v>
+      </c>
+      <c r="L120" t="s">
+        <v>966</v>
       </c>
     </row>
     <row r="121" spans="2:12">
       <c r="C121" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D121" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E121" t="s">
         <v>427</v>
       </c>
       <c r="G121" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="I121" t="s">
-        <v>781</v>
+        <v>786</v>
       </c>
       <c r="J121" t="s">
-        <v>870</v>
+        <v>865</v>
       </c>
       <c r="K121" t="s">
-        <v>934</v>
+        <v>929</v>
       </c>
     </row>
     <row r="122" spans="2:12">
       <c r="C122" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D122" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E122" t="s">
         <v>427</v>
       </c>
       <c r="G122" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="I122" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
       <c r="J122" t="s">
-        <v>880</v>
+        <v>871</v>
       </c>
       <c r="K122" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
     </row>
     <row r="123" spans="2:12">
       <c r="C123" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D123" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E123" t="s">
         <v>427</v>
       </c>
       <c r="G123" t="s">
-        <v>596</v>
-      </c>
-      <c r="H123" t="s">
-        <v>713</v>
+        <v>597</v>
       </c>
       <c r="I123" t="s">
         <v>787</v>
       </c>
       <c r="J123" t="s">
-        <v>866</v>
+        <v>881</v>
       </c>
       <c r="K123" t="s">
-        <v>931</v>
-      </c>
-      <c r="L123" t="s">
-        <v>967</v>
+        <v>935</v>
       </c>
     </row>
     <row r="124" spans="2:12">
       <c r="C124" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D124" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E124" t="s">
         <v>427</v>
       </c>
       <c r="G124" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="H124" t="s">
         <v>713</v>
@@ -6583,61 +6583,67 @@
         <v>788</v>
       </c>
       <c r="J124" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="K124" t="s">
         <v>931</v>
       </c>
       <c r="L124" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="125" spans="2:12">
       <c r="C125" t="s">
         <v>151</v>
       </c>
+      <c r="D125" t="s">
+        <v>309</v>
+      </c>
+      <c r="E125" t="s">
+        <v>427</v>
+      </c>
       <c r="G125" t="s">
         <v>597</v>
       </c>
+      <c r="H125" t="s">
+        <v>713</v>
+      </c>
+      <c r="I125" t="s">
+        <v>789</v>
+      </c>
+      <c r="J125" t="s">
+        <v>867</v>
+      </c>
       <c r="K125" t="s">
-        <v>930</v>
+        <v>931</v>
+      </c>
+      <c r="L125" t="s">
+        <v>968</v>
       </c>
     </row>
     <row r="126" spans="2:12">
       <c r="C126" t="s">
         <v>152</v>
       </c>
-      <c r="D126" t="s">
-        <v>309</v>
-      </c>
-      <c r="E126" t="s">
-        <v>427</v>
-      </c>
       <c r="G126" t="s">
         <v>598</v>
       </c>
-      <c r="I126" t="s">
-        <v>789</v>
-      </c>
-      <c r="J126" t="s">
-        <v>881</v>
-      </c>
       <c r="K126" t="s">
         <v>930</v>
       </c>
     </row>
     <row r="127" spans="2:12">
       <c r="C127" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D127" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="E127" t="s">
         <v>427</v>
       </c>
       <c r="G127" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="I127" t="s">
         <v>790</v>
@@ -6646,21 +6652,21 @@
         <v>882</v>
       </c>
       <c r="K127" t="s">
-        <v>934</v>
+        <v>930</v>
       </c>
     </row>
     <row r="128" spans="2:12">
       <c r="C128" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D128" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="E128" t="s">
         <v>427</v>
       </c>
       <c r="G128" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="I128" t="s">
         <v>791</v>
@@ -6669,50 +6675,44 @@
         <v>883</v>
       </c>
       <c r="K128" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
     </row>
     <row r="129" spans="2:12">
       <c r="C129" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D129" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="E129" t="s">
         <v>427</v>
       </c>
       <c r="G129" t="s">
-        <v>598</v>
-      </c>
-      <c r="H129" t="s">
-        <v>714</v>
+        <v>599</v>
       </c>
       <c r="I129" t="s">
         <v>792</v>
       </c>
       <c r="J129" t="s">
-        <v>866</v>
+        <v>884</v>
       </c>
       <c r="K129" t="s">
-        <v>931</v>
-      </c>
-      <c r="L129" t="s">
-        <v>969</v>
+        <v>935</v>
       </c>
     </row>
     <row r="130" spans="2:12">
       <c r="C130" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D130" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="E130" t="s">
         <v>427</v>
       </c>
       <c r="G130" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="H130" t="s">
         <v>714</v>
@@ -6721,13 +6721,13 @@
         <v>793</v>
       </c>
       <c r="J130" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="K130" t="s">
         <v>931</v>
       </c>
       <c r="L130" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="131" spans="2:12">
@@ -6743,66 +6743,69 @@
       <c r="G131" t="s">
         <v>599</v>
       </c>
+      <c r="H131" t="s">
+        <v>714</v>
+      </c>
       <c r="I131" t="s">
         <v>794</v>
       </c>
       <c r="J131" t="s">
-        <v>881</v>
+        <v>867</v>
       </c>
       <c r="K131" t="s">
-        <v>930</v>
+        <v>931</v>
+      </c>
+      <c r="L131" t="s">
+        <v>970</v>
       </c>
     </row>
     <row r="132" spans="2:12">
       <c r="C132" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D132" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="E132" t="s">
         <v>427</v>
       </c>
       <c r="G132" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="I132" t="s">
-        <v>790</v>
+        <v>795</v>
       </c>
       <c r="J132" t="s">
         <v>882</v>
       </c>
       <c r="K132" t="s">
-        <v>934</v>
+        <v>930</v>
       </c>
     </row>
     <row r="133" spans="2:12">
       <c r="C133" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D133" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="E133" t="s">
         <v>427</v>
       </c>
       <c r="G133" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="I133" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="J133" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="K133" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
     </row>
     <row r="134" spans="2:12">
-      <c r="B134" t="s">
-        <v>49</v>
-      </c>
       <c r="C134" t="s">
         <v>154</v>
       </c>
@@ -6810,123 +6813,126 @@
         <v>311</v>
       </c>
       <c r="E134" t="s">
-        <v>446</v>
+        <v>427</v>
       </c>
       <c r="G134" t="s">
         <v>600</v>
       </c>
+      <c r="I134" t="s">
+        <v>796</v>
+      </c>
+      <c r="J134" t="s">
+        <v>885</v>
+      </c>
+      <c r="K134" t="s">
+        <v>935</v>
+      </c>
     </row>
     <row r="135" spans="2:12">
+      <c r="B135" t="s">
+        <v>49</v>
+      </c>
       <c r="C135" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D135" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="E135" t="s">
+        <v>447</v>
+      </c>
+      <c r="G135" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="136" spans="2:12">
+      <c r="C136" t="s">
+        <v>154</v>
+      </c>
+      <c r="D136" t="s">
+        <v>311</v>
+      </c>
+      <c r="E136" t="s">
         <v>427</v>
       </c>
-      <c r="G135" t="s">
-        <v>599</v>
-      </c>
-      <c r="H135" t="s">
+      <c r="G136" t="s">
+        <v>600</v>
+      </c>
+      <c r="H136" t="s">
         <v>715</v>
-      </c>
-      <c r="I135" t="s">
-        <v>796</v>
-      </c>
-      <c r="J135" t="s">
-        <v>866</v>
-      </c>
-      <c r="K135" t="s">
-        <v>931</v>
-      </c>
-      <c r="L135" t="s">
-        <v>971</v>
-      </c>
-    </row>
-    <row r="136" spans="2:12">
-      <c r="B136" t="s">
-        <v>49</v>
-      </c>
-      <c r="C136" t="s">
-        <v>155</v>
-      </c>
-      <c r="D136" t="s">
-        <v>312</v>
-      </c>
-      <c r="E136" t="s">
-        <v>447</v>
-      </c>
-      <c r="G136" t="s">
-        <v>601</v>
-      </c>
-      <c r="H136" t="s">
-        <v>716</v>
       </c>
       <c r="I136" t="s">
         <v>797</v>
       </c>
       <c r="J136" t="s">
-        <v>885</v>
+        <v>866</v>
+      </c>
+      <c r="K136" t="s">
+        <v>931</v>
+      </c>
+      <c r="L136" t="s">
+        <v>971</v>
       </c>
     </row>
     <row r="137" spans="2:12">
+      <c r="B137" t="s">
+        <v>49</v>
+      </c>
       <c r="C137" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="D137" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="E137" t="s">
-        <v>427</v>
+        <v>448</v>
       </c>
       <c r="G137" t="s">
-        <v>599</v>
+        <v>602</v>
       </c>
       <c r="H137" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="I137" t="s">
         <v>798</v>
       </c>
       <c r="J137" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="138" spans="2:12">
+      <c r="C138" t="s">
+        <v>154</v>
+      </c>
+      <c r="D138" t="s">
+        <v>311</v>
+      </c>
+      <c r="E138" t="s">
+        <v>427</v>
+      </c>
+      <c r="G138" t="s">
+        <v>600</v>
+      </c>
+      <c r="H138" t="s">
+        <v>715</v>
+      </c>
+      <c r="I138" t="s">
+        <v>799</v>
+      </c>
+      <c r="J138" t="s">
         <v>867</v>
       </c>
-      <c r="K137" t="s">
+      <c r="K138" t="s">
         <v>931</v>
       </c>
-      <c r="L137" t="s">
+      <c r="L138" t="s">
         <v>972</v>
       </c>
     </row>
-    <row r="138" spans="2:12">
-      <c r="B138" t="s">
+    <row r="139" spans="2:12">
+      <c r="B139" t="s">
         <v>49</v>
       </c>
-      <c r="C138" t="s">
-        <v>156</v>
-      </c>
-      <c r="D138" t="s">
-        <v>313</v>
-      </c>
-      <c r="E138" t="s">
-        <v>448</v>
-      </c>
-      <c r="G138" t="s">
-        <v>602</v>
-      </c>
-      <c r="H138" t="s">
-        <v>716</v>
-      </c>
-      <c r="I138" t="s">
-        <v>797</v>
-      </c>
-      <c r="J138" t="s">
-        <v>886</v>
-      </c>
-    </row>
-    <row r="139" spans="2:12">
       <c r="C139" t="s">
         <v>157</v>
       </c>
@@ -6934,25 +6940,22 @@
         <v>314</v>
       </c>
       <c r="E139" t="s">
-        <v>427</v>
+        <v>449</v>
       </c>
       <c r="G139" t="s">
         <v>603</v>
       </c>
+      <c r="H139" t="s">
+        <v>716</v>
+      </c>
       <c r="I139" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="J139" t="s">
-        <v>881</v>
-      </c>
-      <c r="K139" t="s">
-        <v>930</v>
+        <v>887</v>
       </c>
     </row>
     <row r="140" spans="2:12">
-      <c r="B140" t="s">
-        <v>49</v>
-      </c>
       <c r="C140" t="s">
         <v>158</v>
       </c>
@@ -6960,7 +6963,7 @@
         <v>315</v>
       </c>
       <c r="E140" t="s">
-        <v>449</v>
+        <v>427</v>
       </c>
       <c r="G140" t="s">
         <v>604</v>
@@ -6969,7 +6972,10 @@
         <v>800</v>
       </c>
       <c r="J140" t="s">
-        <v>887</v>
+        <v>882</v>
+      </c>
+      <c r="K140" t="s">
+        <v>930</v>
       </c>
     </row>
     <row r="141" spans="2:12">
@@ -6988,9 +6994,6 @@
       <c r="G141" t="s">
         <v>605</v>
       </c>
-      <c r="H141" t="s">
-        <v>717</v>
-      </c>
       <c r="I141" t="s">
         <v>801</v>
       </c>
@@ -6999,119 +7002,131 @@
       </c>
     </row>
     <row r="142" spans="2:12">
+      <c r="B142" t="s">
+        <v>49</v>
+      </c>
       <c r="C142" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D142" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="E142" t="s">
-        <v>427</v>
+        <v>451</v>
       </c>
       <c r="G142" t="s">
-        <v>603</v>
+        <v>606</v>
       </c>
       <c r="H142" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="I142" t="s">
         <v>802</v>
       </c>
       <c r="J142" t="s">
-        <v>866</v>
-      </c>
-      <c r="K142" t="s">
-        <v>931</v>
-      </c>
-      <c r="L142" t="s">
-        <v>973</v>
+        <v>889</v>
       </c>
     </row>
     <row r="143" spans="2:12">
-      <c r="B143" t="s">
-        <v>49</v>
-      </c>
       <c r="C143" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D143" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E143" t="s">
-        <v>451</v>
+        <v>427</v>
       </c>
       <c r="G143" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="H143" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="I143" t="s">
         <v>803</v>
       </c>
       <c r="J143" t="s">
-        <v>889</v>
+        <v>866</v>
+      </c>
+      <c r="K143" t="s">
+        <v>931</v>
+      </c>
+      <c r="L143" t="s">
+        <v>973</v>
       </c>
     </row>
     <row r="144" spans="2:12">
+      <c r="B144" t="s">
+        <v>49</v>
+      </c>
       <c r="C144" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="D144" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="E144" t="s">
-        <v>427</v>
+        <v>452</v>
       </c>
       <c r="G144" t="s">
-        <v>603</v>
+        <v>607</v>
       </c>
       <c r="H144" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="I144" t="s">
         <v>804</v>
       </c>
       <c r="J144" t="s">
-        <v>867</v>
-      </c>
-      <c r="K144" t="s">
-        <v>931</v>
-      </c>
-      <c r="L144" t="s">
-        <v>974</v>
+        <v>890</v>
       </c>
     </row>
     <row r="145" spans="1:12">
-      <c r="A145" t="s">
-        <v>49</v>
-      </c>
-      <c r="B145" t="s">
-        <v>49</v>
-      </c>
       <c r="C145" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D145" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="E145" t="s">
-        <v>452</v>
+        <v>427</v>
       </c>
       <c r="G145" t="s">
-        <v>607</v>
+        <v>604</v>
+      </c>
+      <c r="H145" t="s">
+        <v>718</v>
       </c>
       <c r="I145" t="s">
         <v>805</v>
       </c>
       <c r="J145" t="s">
-        <v>890</v>
+        <v>867</v>
+      </c>
+      <c r="K145" t="s">
+        <v>931</v>
+      </c>
+      <c r="L145" t="s">
+        <v>974</v>
       </c>
     </row>
     <row r="146" spans="1:12">
+      <c r="A146" t="s">
+        <v>49</v>
+      </c>
+      <c r="B146" t="s">
+        <v>49</v>
+      </c>
       <c r="C146" t="s">
         <v>162</v>
       </c>
+      <c r="D146" t="s">
+        <v>319</v>
+      </c>
+      <c r="E146" t="s">
+        <v>453</v>
+      </c>
       <c r="G146" t="s">
         <v>608</v>
       </c>
@@ -7121,26 +7136,11 @@
       <c r="J146" t="s">
         <v>891</v>
       </c>
-      <c r="K146" t="s">
-        <v>929</v>
-      </c>
     </row>
     <row r="147" spans="1:12">
-      <c r="A147" t="s">
-        <v>49</v>
-      </c>
-      <c r="B147" t="s">
-        <v>49</v>
-      </c>
       <c r="C147" t="s">
         <v>163</v>
       </c>
-      <c r="D147" t="s">
-        <v>319</v>
-      </c>
-      <c r="E147" t="s">
-        <v>453</v>
-      </c>
       <c r="G147" t="s">
         <v>609</v>
       </c>
@@ -7150,8 +7150,14 @@
       <c r="J147" t="s">
         <v>892</v>
       </c>
+      <c r="K147" t="s">
+        <v>929</v>
+      </c>
     </row>
     <row r="148" spans="1:12">
+      <c r="A148" t="s">
+        <v>49</v>
+      </c>
       <c r="B148" t="s">
         <v>49</v>
       </c>
@@ -7175,8 +7181,8 @@
       </c>
     </row>
     <row r="149" spans="1:12">
-      <c r="A149" t="s">
-        <v>20</v>
+      <c r="B149" t="s">
+        <v>49</v>
       </c>
       <c r="C149" t="s">
         <v>165</v>
@@ -7196,11 +7202,11 @@
       <c r="J149" t="s">
         <v>894</v>
       </c>
-      <c r="K149" t="s">
-        <v>935</v>
-      </c>
     </row>
     <row r="150" spans="1:12">
+      <c r="A150" t="s">
+        <v>20</v>
+      </c>
       <c r="C150" t="s">
         <v>166</v>
       </c>
@@ -7208,7 +7214,7 @@
         <v>322</v>
       </c>
       <c r="E150" t="s">
-        <v>455</v>
+        <v>428</v>
       </c>
       <c r="G150" t="s">
         <v>612</v>
@@ -7217,16 +7223,13 @@
         <v>810</v>
       </c>
       <c r="J150" t="s">
-        <v>834</v>
+        <v>895</v>
       </c>
       <c r="K150" t="s">
         <v>933</v>
       </c>
     </row>
     <row r="151" spans="1:12">
-      <c r="B151" t="s">
-        <v>49</v>
-      </c>
       <c r="C151" t="s">
         <v>167</v>
       </c>
@@ -7234,7 +7237,7 @@
         <v>323</v>
       </c>
       <c r="E151" t="s">
-        <v>456</v>
+        <v>428</v>
       </c>
       <c r="G151" t="s">
         <v>613</v>
@@ -7243,42 +7246,45 @@
         <v>811</v>
       </c>
       <c r="J151" t="s">
-        <v>895</v>
+        <v>834</v>
+      </c>
+      <c r="K151" t="s">
+        <v>934</v>
       </c>
     </row>
     <row r="152" spans="1:12">
+      <c r="B152" t="s">
+        <v>49</v>
+      </c>
       <c r="C152" t="s">
         <v>168</v>
       </c>
+      <c r="D152" t="s">
+        <v>324</v>
+      </c>
+      <c r="E152" t="s">
+        <v>456</v>
+      </c>
       <c r="G152" t="s">
         <v>614</v>
       </c>
-      <c r="H152" t="s">
-        <v>719</v>
-      </c>
       <c r="I152" t="s">
         <v>812</v>
       </c>
       <c r="J152" t="s">
         <v>896</v>
-      </c>
-      <c r="K152" t="s">
-        <v>929</v>
       </c>
     </row>
     <row r="153" spans="1:12">
       <c r="C153" t="s">
         <v>169</v>
       </c>
-      <c r="D153" t="s">
-        <v>324</v>
-      </c>
-      <c r="E153" t="s">
-        <v>457</v>
-      </c>
       <c r="G153" t="s">
         <v>615</v>
       </c>
+      <c r="H153" t="s">
+        <v>719</v>
+      </c>
       <c r="I153" t="s">
         <v>813</v>
       </c>
@@ -7287,9 +7293,6 @@
       </c>
       <c r="K153" t="s">
         <v>929</v>
-      </c>
-      <c r="L153" t="s">
-        <v>975</v>
       </c>
     </row>
     <row r="154" spans="1:12">
@@ -7300,7 +7303,7 @@
         <v>325</v>
       </c>
       <c r="E154" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G154" t="s">
         <v>616</v>
@@ -7319,69 +7322,69 @@
       </c>
     </row>
     <row r="155" spans="1:12">
-      <c r="A155" t="s">
-        <v>20</v>
-      </c>
       <c r="C155" t="s">
         <v>171</v>
       </c>
+      <c r="D155" t="s">
+        <v>326</v>
+      </c>
+      <c r="E155" t="s">
+        <v>458</v>
+      </c>
       <c r="G155" t="s">
         <v>617</v>
       </c>
-      <c r="H155" t="s">
-        <v>720</v>
-      </c>
       <c r="I155" t="s">
-        <v>812</v>
+        <v>815</v>
       </c>
       <c r="J155" t="s">
-        <v>896</v>
+        <v>899</v>
       </c>
       <c r="K155" t="s">
-        <v>935</v>
+        <v>929</v>
+      </c>
+      <c r="L155" t="s">
+        <v>975</v>
       </c>
     </row>
     <row r="156" spans="1:12">
+      <c r="A156" t="s">
+        <v>20</v>
+      </c>
       <c r="C156" t="s">
         <v>172</v>
       </c>
       <c r="G156" t="s">
         <v>618</v>
       </c>
+      <c r="H156" t="s">
+        <v>720</v>
+      </c>
       <c r="I156" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="J156" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="K156" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
     </row>
     <row r="157" spans="1:12">
-      <c r="A157" t="s">
-        <v>49</v>
-      </c>
       <c r="C157" t="s">
         <v>173</v>
       </c>
-      <c r="D157" t="s">
-        <v>326</v>
-      </c>
-      <c r="E157" t="s">
-        <v>455</v>
-      </c>
       <c r="G157" t="s">
         <v>619</v>
       </c>
       <c r="I157" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="J157" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="K157" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
     </row>
     <row r="158" spans="1:12">
@@ -7398,7 +7401,7 @@
         <v>620</v>
       </c>
       <c r="I158" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="J158" t="s">
         <v>900</v>
@@ -7441,7 +7444,7 @@
         <v>622</v>
       </c>
       <c r="K160" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
     </row>
     <row r="161" spans="1:12">
@@ -7475,7 +7478,7 @@
         <v>624</v>
       </c>
       <c r="K162" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
     </row>
     <row r="163" spans="1:12">
@@ -7526,7 +7529,7 @@
         <v>627</v>
       </c>
       <c r="K165" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
     </row>
     <row r="166" spans="1:12">
@@ -7557,7 +7560,7 @@
         <v>629</v>
       </c>
       <c r="K167" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
     </row>
     <row r="168" spans="1:12">
@@ -7568,7 +7571,7 @@
         <v>630</v>
       </c>
       <c r="K168" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
     </row>
     <row r="169" spans="1:12">
@@ -7662,7 +7665,7 @@
         <v>635</v>
       </c>
       <c r="K173" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
     </row>
     <row r="174" spans="1:12">
@@ -7716,7 +7719,7 @@
         <v>638</v>
       </c>
       <c r="K176" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
     </row>
     <row r="177" spans="1:12">
@@ -7767,7 +7770,7 @@
         <v>641</v>
       </c>
       <c r="K179" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
     </row>
     <row r="180" spans="1:12">
@@ -7864,16 +7867,16 @@
         <v>345</v>
       </c>
       <c r="E184" t="s">
-        <v>455</v>
+        <v>428</v>
       </c>
       <c r="G184" t="s">
         <v>646</v>
       </c>
       <c r="I184" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="J184" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
     </row>
     <row r="185" spans="1:12">
@@ -7884,13 +7887,13 @@
         <v>346</v>
       </c>
       <c r="E185" t="s">
-        <v>455</v>
+        <v>428</v>
       </c>
       <c r="G185" t="s">
         <v>647</v>
       </c>
       <c r="I185" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="J185" t="s">
         <v>901</v>
@@ -8020,7 +8023,7 @@
         <v>652</v>
       </c>
       <c r="I190" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="J190" t="s">
         <v>907</v>
@@ -8040,7 +8043,7 @@
         <v>653</v>
       </c>
       <c r="I191" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="J191" t="s">
         <v>908</v>
@@ -8060,7 +8063,7 @@
         <v>654</v>
       </c>
       <c r="I192" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="J192" t="s">
         <v>909</v>
@@ -8086,7 +8089,7 @@
         <v>735</v>
       </c>
       <c r="J193" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
     </row>
     <row r="194" spans="1:12">
@@ -8155,7 +8158,7 @@
         <v>735</v>
       </c>
       <c r="J196" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
     </row>
     <row r="197" spans="1:12">
@@ -8238,7 +8241,7 @@
         <v>360</v>
       </c>
       <c r="E200" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="F200" t="s">
         <v>489</v>
@@ -8247,7 +8250,7 @@
         <v>662</v>
       </c>
       <c r="I200" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="J200" t="s">
         <v>913</v>
@@ -8399,7 +8402,7 @@
         <v>367</v>
       </c>
       <c r="E207" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="F207" t="s">
         <v>488</v>
@@ -8408,7 +8411,7 @@
         <v>669</v>
       </c>
       <c r="I207" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="J207" t="s">
         <v>920</v>
@@ -8714,7 +8717,7 @@
         <v>687</v>
       </c>
       <c r="I225" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="J225" t="s">
         <v>865</v>
@@ -8734,7 +8737,7 @@
         <v>688</v>
       </c>
       <c r="I226" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="J226" t="s">
         <v>865</v>
@@ -8757,7 +8760,7 @@
         <v>721</v>
       </c>
       <c r="I227" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="J227" t="s">
         <v>867</v>
@@ -8780,7 +8783,7 @@
         <v>721</v>
       </c>
       <c r="I228" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="J228" t="s">
         <v>867</v>
@@ -8823,10 +8826,10 @@
         <v>692</v>
       </c>
       <c r="I230" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="J230" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
     </row>
     <row r="231" spans="3:10">
@@ -8843,10 +8846,10 @@
         <v>693</v>
       </c>
       <c r="I231" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="J231" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
     </row>
     <row r="232" spans="3:10">
@@ -8863,10 +8866,10 @@
         <v>694</v>
       </c>
       <c r="I232" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="J232" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
     </row>
     <row r="233" spans="3:10">
@@ -8883,7 +8886,7 @@
         <v>695</v>
       </c>
       <c r="I233" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="J233" t="s">
         <v>865</v>
@@ -8906,7 +8909,7 @@
         <v>707</v>
       </c>
       <c r="I234" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="J234" t="s">
         <v>865</v>
@@ -9038,7 +9041,7 @@
         <v>991</v>
       </c>
       <c r="C10" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -9060,7 +9063,7 @@
         <v>993</v>
       </c>
       <c r="C12" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
     </row>
     <row r="13" spans="1:5">

</xml_diff>